<commit_message>
Added wireframe link and image;updated blog
</commit_message>
<xml_diff>
--- a/blog.xlsx
+++ b/blog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26707"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjang\Documents\GitHub\PollsPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA22122-45F7-4612-BC01-B721FB420BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DFA22122-45F7-4612-BC01-B721FB420BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC5F7B37-3C9C-4656-87FC-433F2866B717}"/>
   <bookViews>
     <workbookView xWindow="27330" yWindow="1410" windowWidth="19635" windowHeight="18105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Team member</t>
   </si>
@@ -86,29 +86,35 @@
     <t>meeting in class</t>
   </si>
   <si>
+    <t>discuss system structure</t>
+  </si>
+  <si>
     <t>documents for DB diagram, use-case diagram, blog etc.</t>
   </si>
   <si>
+    <t>DB diagram work</t>
+  </si>
+  <si>
+    <t>UML diagram work</t>
+  </si>
+  <si>
+    <t>Wire frame work</t>
+  </si>
+  <si>
+    <t>wire frame draft</t>
+  </si>
+  <si>
+    <t>Milestone 2</t>
+  </si>
+  <si>
     <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>DB diagram work</t>
-  </si>
-  <si>
-    <t>UML diagram work</t>
-  </si>
-  <si>
-    <t>Milestone 2</t>
-  </si>
-  <si>
-    <t>discuss system structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,15 +456,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -474,6 +489,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -482,66 +506,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,10 +854,10 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="6" width="9.140625" style="1"/>
@@ -874,16 +868,16 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -900,38 +894,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A6" s="33"/>
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -947,694 +941,338 @@
       <c r="F6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="38"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="G6" s="39"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13">
         <v>45118</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="1">
         <v>3</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="9"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13">
+        <v>45118</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13">
+        <v>45118</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13">
+        <v>45118</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
-        <v>45118</v>
-      </c>
-      <c r="B10" s="39">
-        <v>1</v>
-      </c>
-      <c r="C10" s="39">
-        <v>0</v>
-      </c>
-      <c r="D10" s="39">
-        <v>0</v>
-      </c>
-      <c r="E10" s="39">
-        <v>0</v>
-      </c>
-      <c r="F10" s="39">
-        <v>0</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="39">
-        <v>4</v>
-      </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="29"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
-        <v>45118</v>
-      </c>
-      <c r="B11" s="39">
-        <v>1</v>
-      </c>
-      <c r="C11" s="39">
-        <v>0</v>
-      </c>
-      <c r="D11" s="39">
-        <v>0</v>
-      </c>
-      <c r="E11" s="39">
-        <v>0</v>
-      </c>
-      <c r="F11" s="39">
-        <v>0</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="39">
-        <v>2</v>
-      </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="29"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="9"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="9"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="9"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="9"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="9"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="9"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="9"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="9"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="9"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
+      <c r="A22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="9"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="9"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="9"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
+      <c r="A26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="9"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="9"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="9"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="9"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="9"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="9"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="9"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="9"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="9"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="9"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="9"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="9"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="9"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="9"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="9"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="9"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="9"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="9"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="9"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="9"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="9"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="9"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="9"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="9"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="9"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="9"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="9"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="9"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="9"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
       <c r="J55" s="8"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="9"/>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="9"/>
-      <c r="B57" s="41"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="9"/>
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="10"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>

</xml_diff>

<commit_message>
deleted .html diagrams and added .sql script in backend folder
</commit_message>
<xml_diff>
--- a/blog.xlsx
+++ b/blog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26707"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjang\Documents\GitHub\PollsPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DFA22122-45F7-4612-BC01-B721FB420BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC5F7B37-3C9C-4656-87FC-433F2866B717}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198AA9E9-D2C7-40F3-9E14-E5400255BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27330" yWindow="1410" windowWidth="19635" windowHeight="18105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Team member</t>
   </si>
@@ -108,13 +108,19 @@
   </si>
   <si>
     <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>DB script work</t>
+  </si>
+  <si>
+    <t>.sql script</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,9 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,10 +860,10 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="6" width="9.140625" style="1"/>
@@ -868,16 +874,16 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -894,38 +900,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A5" s="32" t="s">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="38" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
@@ -941,27 +947,27 @@
       <c r="F6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="35"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="27" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="13">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="39">
         <v>45118</v>
       </c>
       <c r="B8" s="1">
@@ -985,20 +991,20 @@
       <c r="H8" s="1">
         <v>3</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="9"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="13">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
         <v>45118</v>
       </c>
       <c r="B10" s="1">
@@ -1024,8 +1030,8 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
         <v>45118</v>
       </c>
       <c r="B11" s="1">
@@ -1051,13 +1057,25 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="13">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
         <v>45118</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1068,211 +1086,236 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="9"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="9"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
+        <v>45120</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="9"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="J55" s="8"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>

</xml_diff>

<commit_message>
updated blog and deleted .DS_Store
</commit_message>
<xml_diff>
--- a/blog.xlsx
+++ b/blog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16300b0c7e6b1157/Bureau/McGill1/CapstoneProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjang\Documents\GitHub\PollsPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8B9567C-524B-404A-8E42-24C88EEC4564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95891CC-2681-407F-B991-4D88FE7D0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27330" yWindow="1410" windowWidth="19635" windowHeight="18105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Team member</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Server work</t>
+  </si>
+  <si>
+    <t>Troubleshooting</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>DB connection issues with front-end for Olivier</t>
   </si>
 </sst>
 </file>
@@ -904,22 +913,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="21" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.1796875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -928,7 +937,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -945,13 +954,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="26"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
@@ -975,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36"/>
       <c r="B6" s="5" t="s">
         <v>1</v>
@@ -997,7 +1006,7 @@
       <c r="I6" s="40"/>
       <c r="J6" s="38"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>15</v>
       </c>
@@ -1011,7 +1020,7 @@
       <c r="I7" s="31"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>45118</v>
       </c>
@@ -1043,12 +1052,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="I9" s="33"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>45118</v>
       </c>
@@ -1075,7 +1084,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>45118</v>
       </c>
@@ -1102,7 +1111,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>45118</v>
       </c>
@@ -1131,7 +1140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>45118</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>45120</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>45120</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>45120</v>
       </c>
@@ -1251,7 +1260,7 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>45121</v>
       </c>
@@ -1281,7 +1290,7 @@
       </c>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>45121</v>
       </c>
@@ -1311,7 +1320,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>45122</v>
       </c>
@@ -1341,19 +1350,47 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>45123</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
@@ -1367,19 +1404,19 @@
       <c r="I23" s="18"/>
       <c r="J23" s="19"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>24</v>
       </c>
@@ -1393,135 +1430,135 @@
       <c r="I27" s="21"/>
       <c r="J27" s="22"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="J55" s="8"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="J56" s="8"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="J59" s="8"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>

</xml_diff>